<commit_message>
dar biski pataisyta linux
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -22,12 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Cia kazkas parasyta</t>
   </si>
   <si>
     <t xml:space="preserve">Cia irgi kazkas parasyta Linux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NU tarkim dar kazkas</t>
   </si>
 </sst>
 </file>
@@ -157,10 +160,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -171,6 +174,11 @@
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Paptaisytas pirmas lapas WIndows
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Cia kazkas parasyta</t>
+  </si>
+  <si>
+    <t>Cia dar kazkas prasyta Windows</t>
   </si>
 </sst>
 </file>
@@ -357,15 +360,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>